<commit_message>
Actualización para incluir posdoc Minciencias y otra info
</commit_message>
<xml_diff>
--- a/data/experiencia_docente.xlsx
+++ b/data/experiencia_docente.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFE0B6E-E72E-4BBB-B7CD-ECB77B2C7D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662FBEA8-59EC-45BE-8BA0-C2C5CF5D1639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>what</t>
   </si>
@@ -54,15 +54,6 @@
     <t>Universidad Central</t>
   </si>
   <si>
-    <t>2017 - Actualmente</t>
-  </si>
-  <si>
-    <t>Gestión de la comunicación (4 horas semanales - 2018 - Actualmente)</t>
-  </si>
-  <si>
-    <t>Prácticas profesionales (4 horas semanales - 2022 - Actualmente)</t>
-  </si>
-  <si>
     <t>Opción de grado Comunicación y DDHH - módulo Comunicación y Género (4 horas semanales - 2019 - 2021)</t>
   </si>
   <si>
@@ -82,6 +73,30 @@
   </si>
   <si>
     <t>Proyecto de línea - investigación (4 horas semanales - 2018)</t>
+  </si>
+  <si>
+    <t>2017 - 2023</t>
+  </si>
+  <si>
+    <t>Posdoctorado</t>
+  </si>
+  <si>
+    <t>Desde 2023</t>
+  </si>
+  <si>
+    <t>Asociación Red de Mujeres Víctimas y Profesionales</t>
+  </si>
+  <si>
+    <t>\textbf{Proyecto: } La necesidad de generar procesos de reparación social a las mujeres víctimas y sobrevivientes de violencias sexuales en el marco del conflicto armado desde el quehacer periodístico. Diversas propuestas de tratamiento según contextos</t>
+  </si>
+  <si>
+    <t>Financiación del Ministerio de Ciencia Tecnología e Innovación - Minciencias</t>
+  </si>
+  <si>
+    <t>Gestión de la comunicación (4 horas semanales - 2018 - 2023)</t>
+  </si>
+  <si>
+    <t>Prácticas profesionales (4 horas semanales - 2022 - 2023)</t>
   </si>
 </sst>
 </file>
@@ -894,16 +909,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="85.28515625" bestFit="1" customWidth="1"/>
@@ -928,54 +943,76 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>